<commit_message>
Removed papers and added Invader_survival_David
The file only plot the evolution of chemical species.
</commit_message>
<xml_diff>
--- a/Simone_Cavallero/Invaders_Realizations/Code/output/AC_n3.xlsx
+++ b/Simone_Cavallero/Invaders_Realizations/Code/output/AC_n3.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,68 +506,278 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>R7</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>R8</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>W1</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>W2</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>W3</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>EM1</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>EM2</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>EM3</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>X1</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>X2</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>X3</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>X4</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>X5</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>X6</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>X7</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>X8</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Zeroes</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>